<commit_message>
Update Group Member Info
</commit_message>
<xml_diff>
--- a/documents/Project-document.xlsx
+++ b/documents/Project-document.xlsx
@@ -1,28 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView windowWidth="28695" windowHeight="13050" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Group member" sheetId="1" r:id="rId1"/>
     <sheet name="Requiment" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39">
   <si>
     <t>Group 5</t>
   </si>
   <si>
+    <t>STT</t>
+  </si>
+  <si>
     <t>Member</t>
   </si>
   <si>
+    <t>Student code</t>
+  </si>
+  <si>
     <t>Nguyễn Đức Trịnh</t>
   </si>
   <si>
@@ -56,7 +62,31 @@
     <t>Đoàn Công Hậu</t>
   </si>
   <si>
-    <t>STT</t>
+    <t>SE61706</t>
+  </si>
+  <si>
+    <t>1/ Thông tin sách</t>
+  </si>
+  <si>
+    <t>Thông tin sách</t>
+  </si>
+  <si>
+    <t>Tác giả</t>
+  </si>
+  <si>
+    <t>Sách</t>
+  </si>
+  <si>
+    <t>Kệ sách</t>
+  </si>
+  <si>
+    <t>Loại sách</t>
+  </si>
+  <si>
+    <t>Ngôn ngữ sách</t>
+  </si>
+  <si>
+    <t>2/ Chi tiết nhân viên quản lý</t>
   </si>
   <si>
     <t>Số thứ tự</t>
@@ -65,30 +95,6 @@
     <t>Chức năng</t>
   </si>
   <si>
-    <t>Student code</t>
-  </si>
-  <si>
-    <t>Thông tin sách</t>
-  </si>
-  <si>
-    <t>Tác giả</t>
-  </si>
-  <si>
-    <t>Sách</t>
-  </si>
-  <si>
-    <t>Kệ sách</t>
-  </si>
-  <si>
-    <t>Loại sách</t>
-  </si>
-  <si>
-    <t>Ngôn ngữ sách</t>
-  </si>
-  <si>
-    <t>2/ Chi tiết nhân viên quản lý</t>
-  </si>
-  <si>
     <t>Nhập thêm sách</t>
   </si>
   <si>
@@ -126,40 +132,373 @@
   </si>
   <si>
     <t>Nhận Email khi gần hết hạn</t>
-  </si>
-  <si>
-    <t>1/ Thông tin sách</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -167,9 +506,251 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -181,35 +762,58 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
+    <cellStyle name="Note" xfId="9" builtinId="10"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-  </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
 
@@ -229,19 +833,19 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A12:B20" totalsRowShown="0">
   <autoFilter ref="A12:B20"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Số thứ tự" dataDxfId="1"/>
-    <tableColumn id="3" name="Chức năng" dataDxfId="0"/>
+    <tableColumn id="1" name="Số thứ tự"/>
+    <tableColumn id="2" name="Chức năng"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A23:B27" totalsRowShown="0" headerRowDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A23:B27" totalsRowShown="0">
   <autoFilter ref="A23:B27"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Số thứ tự" dataDxfId="3"/>
-    <tableColumn id="3" name="Chức năng" dataDxfId="2"/>
+    <tableColumn id="1" name="Số thứ tự"/>
+    <tableColumn id="2" name="Chức năng"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -301,7 +905,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -336,7 +940,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -539,142 +1143,147 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="2"/>
   <cols>
-    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" customWidth="1"/>
+    <col min="2" max="2" width="16.8571428571429" customWidth="1"/>
+    <col min="3" max="3" width="22.1428571428571" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8">
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9">
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A3:C27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" customWidth="1"/>
-    <col min="3" max="3" width="36.140625" customWidth="1"/>
+    <col min="2" max="2" width="41.7142857142857" customWidth="1"/>
+    <col min="3" max="3" width="36.1428571428571" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -682,7 +1291,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6">
         <v>2</v>
       </c>
@@ -690,7 +1299,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7">
         <v>3</v>
       </c>
@@ -698,7 +1307,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8">
         <v>4</v>
       </c>
@@ -706,7 +1315,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2">
       <c r="A9">
         <v>5</v>
       </c>
@@ -714,140 +1323,141 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1">
       <c r="A11" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
       <c r="A13" s="2">
         <v>1</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
       <c r="A14" s="2">
         <v>2</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
       <c r="A15" s="2">
         <v>3</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
       <c r="A16" s="2">
         <v>4</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" ht="30" spans="1:2">
       <c r="A17" s="2">
         <v>5</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
       <c r="A18" s="2">
         <v>6</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
       <c r="A19" s="2">
         <v>7</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
       <c r="A20" s="2">
         <v>8</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1">
       <c r="A22" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
       <c r="A23" s="2" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
       <c r="A24" s="2">
         <v>1</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25" s="2">
         <v>2</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C25" s="2"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2">
       <c r="A26" s="2">
         <v>3</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
       <c r="A27" s="2">
         <v>4</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
   <tableParts count="3">
+    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
-    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>